<commit_message>
Deploying to gh-pages from  @ 8e59ed41ed0e7fa73e420b6a27b8088b5ee01cc1 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-2-2.xlsx
+++ b/assets/excel/2021_1-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6B9216-05D1-4BA6-96D1-45A7F0BBDA74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6CFF11-31F0-4C4D-B3B9-28B199CAEF62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{E8B70F38-DE1B-4179-B181-7CCB39045086}"/>
   </bookViews>
@@ -220,7 +220,7 @@
     <t>https://www.integrationsmonitoring.niedersachsen.de.</t>
   </si>
   <si>
-    <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2020</t>
+    <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
 </sst>
 </file>
@@ -525,24 +525,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -563,6 +545,24 @@
     </xf>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -885,8 +885,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:R70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +897,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="34" t="s">
         <v>63</v>
       </c>
       <c r="P1"/>
@@ -905,44 +905,44 @@
     </row>
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="35" t="s">
         <v>45</v>
       </c>
       <c r="P3"/>
       <c r="Q3"/>
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="34" t="s">
         <v>46</v>
       </c>
       <c r="P4"/>
       <c r="Q4"/>
     </row>
     <row r="6" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="35"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="44"/>
     </row>
     <row r="7" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="2">
         <v>2005</v>
       </c>
@@ -993,25 +993,25 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1066,7 +1066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>47</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>48</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>49</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>4</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>8</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
@@ -1596,60 +1596,60 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="36">
         <v>6.0308948852878181</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="36">
         <v>5.9493499722251997</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="36">
         <v>5.8394017576491537</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="36">
         <v>5.7644848116803571</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="36">
         <v>5.7823865604433662</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="36">
         <v>5.7828254427666996</v>
       </c>
-      <c r="I20" s="42">
+      <c r="I20" s="36">
         <v>6.000692907470202</v>
       </c>
-      <c r="J20" s="42">
+      <c r="J20" s="36">
         <v>6.2121513317967869</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="36">
         <v>6.6382379982424684</v>
       </c>
-      <c r="L20" s="42">
+      <c r="L20" s="36">
         <v>7.1235141673956832</v>
       </c>
-      <c r="M20" s="42">
+      <c r="M20" s="36">
         <v>8.1927136389006385</v>
       </c>
-      <c r="N20" s="43">
+      <c r="N20" s="37">
         <v>9.0971535006383135</v>
       </c>
-      <c r="O20" s="44">
+      <c r="O20" s="38">
         <v>9.473383408512948</v>
       </c>
-      <c r="P20" s="45">
+      <c r="P20" s="39">
         <v>9.908569051789156</v>
       </c>
-      <c r="Q20" s="45">
+      <c r="Q20" s="39">
         <v>10.345288097463898</v>
       </c>
-      <c r="R20" s="45">
+      <c r="R20" s="39">
         <v>10.5</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>10</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>11</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>12</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>11.838443474047976</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>13</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>14</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>15</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>17</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>18</v>
       </c>
@@ -2126,60 +2126,60 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="42">
+      <c r="C30" s="36">
         <v>7.7449756668341099</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="36">
         <v>7.6782673140599735</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="36">
         <v>7.6330151364889671</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="36">
         <v>7.5102562324904225</v>
       </c>
-      <c r="G30" s="42">
+      <c r="G30" s="36">
         <v>7.4822632139056404</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="36">
         <v>7.5185473867203187</v>
       </c>
-      <c r="I30" s="42">
+      <c r="I30" s="36">
         <v>7.8492675421353759</v>
       </c>
-      <c r="J30" s="42">
+      <c r="J30" s="36">
         <v>8.1265683690775496</v>
       </c>
-      <c r="K30" s="42">
+      <c r="K30" s="36">
         <v>8.6500793919619028</v>
       </c>
-      <c r="L30" s="42">
+      <c r="L30" s="36">
         <v>9.2580059030180522</v>
       </c>
-      <c r="M30" s="42">
+      <c r="M30" s="36">
         <v>10.485112250209868</v>
       </c>
-      <c r="N30" s="43">
+      <c r="N30" s="37">
         <v>11.567185800214581</v>
       </c>
-      <c r="O30" s="44">
+      <c r="O30" s="38">
         <v>12.019150047571964</v>
       </c>
-      <c r="P30" s="45">
+      <c r="P30" s="39">
         <v>12.489737441302816</v>
       </c>
-      <c r="Q30" s="45">
+      <c r="Q30" s="39">
         <v>12.784198026475652</v>
       </c>
-      <c r="R30" s="45">
+      <c r="R30" s="39">
         <v>12.9</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>19</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>20</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>21</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>22</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>23</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>24</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>25</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>26</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>27</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>29</v>
       </c>
@@ -2762,60 +2762,60 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="42" spans="2:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="42">
+      <c r="C42" s="36">
         <v>4.093694564919522</v>
       </c>
-      <c r="D42" s="42">
+      <c r="D42" s="36">
         <v>4.0275101031276535</v>
       </c>
-      <c r="E42" s="42">
+      <c r="E42" s="36">
         <v>3.9798204959991348</v>
       </c>
-      <c r="F42" s="42">
+      <c r="F42" s="36">
         <v>3.9654187710673368</v>
       </c>
-      <c r="G42" s="42">
+      <c r="G42" s="36">
         <v>3.9871780186507984</v>
       </c>
-      <c r="H42" s="42">
+      <c r="H42" s="36">
         <v>4.0154517272393129</v>
       </c>
-      <c r="I42" s="42">
+      <c r="I42" s="36">
         <v>4.1522931366356612</v>
       </c>
-      <c r="J42" s="42">
+      <c r="J42" s="36">
         <v>4.3165968145516311</v>
       </c>
-      <c r="K42" s="42">
+      <c r="K42" s="36">
         <v>4.6605224886375813</v>
       </c>
-      <c r="L42" s="42">
+      <c r="L42" s="36">
         <v>5.1001510983689125</v>
       </c>
-      <c r="M42" s="42">
+      <c r="M42" s="36">
         <v>5.9621675454081817</v>
       </c>
-      <c r="N42" s="43">
+      <c r="N42" s="37">
         <v>6.8089052170111133</v>
       </c>
-      <c r="O42" s="44">
+      <c r="O42" s="38">
         <v>7.0356011026309364</v>
       </c>
-      <c r="P42" s="45">
+      <c r="P42" s="39">
         <v>7.3758821308376685</v>
       </c>
-      <c r="Q42" s="45">
+      <c r="Q42" s="39">
         <v>7.6917564645127614</v>
       </c>
-      <c r="R42" s="45">
+      <c r="R42" s="39">
         <v>7.9</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
         <v>54</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>53</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>55</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
         <v>56</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>57</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>30</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
         <v>31</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>32</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>33</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>34</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
         <v>35</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>36</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
         <v>37</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>38</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>39</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>40</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>41</v>
       </c>
@@ -3716,109 +3716,109 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="60" spans="2:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:18" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="42">
+      <c r="C60" s="36">
         <v>5.0331271897454171</v>
       </c>
-      <c r="D60" s="42">
+      <c r="D60" s="36">
         <v>5.1105896635533181</v>
       </c>
-      <c r="E60" s="42">
+      <c r="E60" s="36">
         <v>5.2164717445985369</v>
       </c>
-      <c r="F60" s="42">
+      <c r="F60" s="36">
         <v>5.2812790205390243</v>
       </c>
-      <c r="G60" s="42">
+      <c r="G60" s="36">
         <v>5.3440608465020816</v>
       </c>
-      <c r="H60" s="42">
+      <c r="H60" s="36">
         <v>5.5018714878075849</v>
       </c>
-      <c r="I60" s="42">
+      <c r="I60" s="36">
         <v>5.8485220043097526</v>
       </c>
-      <c r="J60" s="42">
+      <c r="J60" s="36">
         <v>6.2256035017535387</v>
       </c>
-      <c r="K60" s="42">
+      <c r="K60" s="36">
         <v>6.6110462751574284</v>
       </c>
-      <c r="L60" s="42">
+      <c r="L60" s="36">
         <v>7.2206958795248966</v>
       </c>
-      <c r="M60" s="42">
+      <c r="M60" s="36">
         <v>8.3309830717064823</v>
       </c>
-      <c r="N60" s="43">
+      <c r="N60" s="37">
         <v>9.435569627576907</v>
       </c>
-      <c r="O60" s="44">
+      <c r="O60" s="38">
         <v>9.8521452979327684</v>
       </c>
-      <c r="P60" s="45">
+      <c r="P60" s="39">
         <v>10.303789638831789</v>
       </c>
-      <c r="Q60" s="45">
+      <c r="Q60" s="39">
         <v>10.635585812589063</v>
       </c>
-      <c r="R60" s="45">
+      <c r="R60" s="39">
         <v>10.9</v>
       </c>
     </row>
-    <row r="61" spans="2:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:18" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C61" s="42">
+      <c r="C61" s="36">
         <v>5.772943675126152</v>
       </c>
-      <c r="D61" s="42">
+      <c r="D61" s="36">
         <v>5.7469009487409313</v>
       </c>
-      <c r="E61" s="42">
+      <c r="E61" s="36">
         <v>5.73403311019353</v>
       </c>
-      <c r="F61" s="42">
+      <c r="F61" s="36">
         <v>5.7018634384448239</v>
       </c>
-      <c r="G61" s="42">
+      <c r="G61" s="36">
         <v>5.7213593708517605</v>
       </c>
-      <c r="H61" s="42">
+      <c r="H61" s="36">
         <v>5.7860071608868227</v>
       </c>
-      <c r="I61" s="42">
+      <c r="I61" s="36">
         <v>6.0543823310098093</v>
       </c>
-      <c r="J61" s="42">
+      <c r="J61" s="36">
         <v>6.3256500357694021</v>
       </c>
-      <c r="K61" s="42">
+      <c r="K61" s="36">
         <v>6.7477699610515751</v>
       </c>
-      <c r="L61" s="42">
+      <c r="L61" s="36">
         <v>7.2953499535374817</v>
       </c>
-      <c r="M61" s="42">
+      <c r="M61" s="36">
         <v>8.3745500434675701</v>
       </c>
-      <c r="N61" s="43">
+      <c r="N61" s="37">
         <v>9.3784865622032587</v>
       </c>
-      <c r="O61" s="44">
+      <c r="O61" s="38">
         <v>9.7561465695062335</v>
       </c>
-      <c r="P61" s="45">
+      <c r="P61" s="39">
         <v>10.18584774996342</v>
       </c>
-      <c r="Q61" s="45">
+      <c r="Q61" s="39">
         <v>10.522970353312298</v>
       </c>
-      <c r="R61" s="45">
+      <c r="R61" s="39">
         <v>10.7</v>
       </c>
     </row>
@@ -3900,22 +3900,22 @@
     </row>
     <row r="66" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="37" t="s">
+      <c r="B67" s="31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="68" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="37" t="s">
+      <c r="B68" s="31" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="69" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="70" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="38" t="s">
+      <c r="B70" s="32" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>